<commit_message>
extended excel parser draft
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shukhovvg\Desktop\Guardian\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shukhovvg\ExcelToJira\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,16 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
-  <si>
-    <t>Summary</t>
-  </si>
-  <si>
-    <t>Labels</t>
-  </si>
-  <si>
-    <t>Tests Stories</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>chat, acceptance</t>
   </si>
@@ -54,6 +45,9 @@
   </si>
   <si>
     <t>test_3</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -375,7 +369,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -385,7 +379,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -396,35 +390,29 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small changes with ExcelParser
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -24,30 +24,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
-  <si>
-    <t>chat</t>
-  </si>
-  <si>
-    <t>test_1</t>
-  </si>
-  <si>
-    <t>test_2</t>
-  </si>
-  <si>
-    <t>test_3</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>chat,acceptance,smoke</t>
   </si>
   <si>
-    <t>GRD-312,GRD-313</t>
-  </si>
-  <si>
     <t>chat,acceptance</t>
   </si>
   <si>
-    <t>GRD-312,GRD-314</t>
+    <t>Loudspeaker: move phone to ear to switch OFF loudspeaker</t>
+  </si>
+  <si>
+    <t>Loudspeaker: move phone from ear to switch back ON loudspeaker</t>
+  </si>
+  <si>
+    <t>Loudspeaker: check on different volume that ON-OFF transition of loudspeaker doesn't affect the volume</t>
+  </si>
+  <si>
+    <t>GRD-342,GRD-343</t>
   </si>
 </sst>
 </file>
@@ -72,7 +66,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -80,12 +74,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,45 +381,46 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="32.85546875" customWidth="1"/>
+    <col min="1" max="1" width="57" customWidth="1"/>
+    <col min="2" max="3" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
+      <c r="A1" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
selecting priority bug fixed
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -24,24 +24,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
-  <si>
-    <t>chat,acceptance,smoke</t>
-  </si>
-  <si>
-    <t>chat,acceptance</t>
-  </si>
-  <si>
-    <t>Loudspeaker: move phone to ear to switch OFF loudspeaker</t>
-  </si>
-  <si>
-    <t>Loudspeaker: move phone from ear to switch back ON loudspeaker</t>
-  </si>
-  <si>
-    <t>Loudspeaker: check on different volume that ON-OFF transition of loudspeaker doesn't affect the volume</t>
-  </si>
-  <si>
-    <t>GRD-342,GRD-343</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>Get patient's details: patient requests patient details</t>
+  </si>
+  <si>
+    <t>Carer confirmation: patient adds to his list not existing in DB carer</t>
+  </si>
+  <si>
+    <t>Carer confirmation: carer added new patient, patient confirmes carer</t>
+  </si>
+  <si>
+    <t>User activation: inactive patient log in to app</t>
+  </si>
+  <si>
+    <t>User activation: inactive carer log in to app</t>
+  </si>
+  <si>
+    <t>GRD-713</t>
   </si>
 </sst>
 </file>
@@ -66,7 +69,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -74,30 +77,16 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,49 +367,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57" customWidth="1"/>
+    <col min="1" max="1" width="107.42578125" customWidth="1"/>
     <col min="2" max="3" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>